<commit_message>
First addition to literature excel
</commit_message>
<xml_diff>
--- a/literature/literature_WB_project.xlsx
+++ b/literature/literature_WB_project.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/cijensen_calpoly_edu/Documents/MSQE/GSE_580/GSE-580-project/literature/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="70" documentId="11_F25DC773A252ABDACC104829C15D7DF45BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E580A4EB-F77E-46AD-B8B3-426214F57C58}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,11 +24,99 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Hypothesis/Question</t>
+  </si>
+  <si>
+    <t>Data Sets</t>
+  </si>
+  <si>
+    <t>Methodology</t>
+  </si>
+  <si>
+    <t>Contribution to Literature</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Monthly Labor Review</t>
+  </si>
+  <si>
+    <t>The NAICS 2022 update and its effect on BLS employment estimates in the retail trade sector</t>
+  </si>
+  <si>
+    <t>Federal Committee on Statistical Methodology</t>
+  </si>
+  <si>
+    <t>Converting Historical Industry Time Series Data from SIC to NAICS</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Robert E. Yuskavage</t>
+  </si>
+  <si>
+    <t>Shane Haley and Kennedy Keller</t>
+  </si>
+  <si>
+    <t>DO INDUSTRIAL CLASSIFICATIONS NEED RE-INVENTING? AN ANALYSIS OF THE RELEVANCE OF THE u.s. SIC SYSTEM FOR PRODUCTIVITY RESEARCH</t>
+  </si>
+  <si>
+    <t>PROCEEDINGS OF THE 6th ASIS SIGICR CLASSIFICAnON RESEARCH WORKSHOP</t>
+  </si>
+  <si>
+    <t>Jack E. Triplett, D. Mark Kennet, Ron Jarmin, and Frank M. Gollop</t>
+  </si>
+  <si>
+    <t>Progress Toward Completing Historical Production Accounts using the North American Industry Classification System</t>
+  </si>
+  <si>
+    <t>Michael J. Harper (BLS), Barbara M. Fraumeni (BEA), Susan G. Powers (BLS), and Robert E. Yuskavage (BEA)</t>
+  </si>
+  <si>
+    <t>Federal Economic Statistics Advisory Committee</t>
+  </si>
+  <si>
+    <t>CREATING A HISTORICAL BRIDGE FOR MANUFACTURING BETWEEN THE STANDARD INDUSTRIAL CLASSIFICATION SYSTEM AND THE NORTH AMERICAN INDUSTRY CLASSIFICATION SYSTEM</t>
+  </si>
+  <si>
+    <t>Kimberly N. Bayard and Shawn D. Klimek</t>
+  </si>
+  <si>
+    <t>Board of Governors of the Federal Reserve and the U.S. Census Bureau</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -49,8 +143,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -66,6 +167,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +435,145 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" customWidth="1"/>
+    <col min="6" max="6" width="28.90625" customWidth="1"/>
+    <col min="7" max="7" width="29.26953125" customWidth="1"/>
+    <col min="8" max="8" width="38.81640625" customWidth="1"/>
+    <col min="9" max="9" width="32.1796875" customWidth="1"/>
+    <col min="10" max="10" width="41.7265625" customWidth="1"/>
+    <col min="11" max="11" width="38.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="101" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>2023</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>2007</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>1995</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>2005</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>2003</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 4 of 5 sources, not perfect but good for now
</commit_message>
<xml_diff>
--- a/literature/literature_WB_project.xlsx
+++ b/literature/literature_WB_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/cijensen_calpoly_edu/Documents/MSQE/GSE_580/GSE-580-project/literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_F25DC773A252ABDACC104829C15D7DF45BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E580A4EB-F77E-46AD-B8B3-426214F57C58}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="11_F25DC773A252ABDACC104829C15D7DF45BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF58544D-F505-4FC7-9250-912B5285DEEB}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Journal</t>
   </si>
@@ -100,6 +100,78 @@
   </si>
   <si>
     <t>Board of Governors of the Federal Reserve and the U.S. Census Bureau</t>
+  </si>
+  <si>
+    <t>Using the U.S. Bureau of Labor Statistics, Current Employment Statistics survey    they are able to get data to compare the aggregate employment captured by different codes as well as quantify where shifts were from one code to another. Using the NASICS 2017 and 2022 job codes and their correspondence tables they can see changes in the codes and where employment will now be classified instead.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The authors use the correspondence tables as well as employment survey data to show trends in employment catagorization across the different classification methods </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the retail sector, the new NASICS classifications reflect the shift in businesses being involved both in online and brick and mortar retailing.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">While three 3 digit codes were dropped from 2017-2022, nearly all the jobs classified under them remained in the retail sector. There were significant reclassifications within each three digit code, reflecting shifts in the retail sector, but the vast majority of positions in the retail sector remained coded there. </t>
+  </si>
+  <si>
+    <t>How did the NAICS 2022 update from 2017 reflect the substantial changes in the retail trade sector and how are jobs within those industries classified in the most recent update</t>
+  </si>
+  <si>
+    <t>U.S. Bureau of Labor Statistics, Current Employment Statistics survey                                                   NAICS 2017 and NAICS 2022 job codes</t>
+  </si>
+  <si>
+    <t>How can we convert data from the old SICs method to the NAICS method to improve research on what drives economic growth, particularly in the Information and Commuication Technology industry</t>
+  </si>
+  <si>
+    <t>Output estimates from 1947-1976 and 1987-1997 on a NAICS rather than a SICs system                            NAICS and SICs and their correspondence</t>
+  </si>
+  <si>
+    <t>Use the NAICS and SICs tables to create a correspondence, then extrapolate that correspondence backward and look at how it effects industry GDP accounts</t>
+  </si>
+  <si>
+    <t>Authors created NAICS and SICs correspondence tables and used them to look at the differences in by industry GDP share and how researchers can look at sectors driving GDP growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demonstrates the difficulty of creating correspondence between different classification systems as well as how it can be done and the advantages of completing it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provide researchers with a method of projecting classification methods backwards so that they can have accurate and consistent historical data to use. </t>
+  </si>
+  <si>
+    <t>Does the old U.S. SICs system for classify industry provide relevant data for productivity research?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only about a fifth of the codes were grouped by production methods making the code very challenging to use in research on productivity. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This demonstrates the need to regularly update classification systems as well as to classify properly. It also shows that proper correspondence from system to system and year to year is essential for researchers. </t>
+  </si>
+  <si>
+    <t>(a) U.S. SIC 1987 (b) 1987 Census of Manufacturers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use the census of manufacturers to create an index based on a Cobb-Douglas production function that shows the degree to which the current system uses production method to classify industries. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authors used expert opinion to consider 4 digit job codes and whether they were group by market or production. The then created an index using a Cobb-Douglas production function and ranked codes based on how similar they were to others in their industry to compare with their opinions. The more dissimilar, the more the need for revision. </t>
+  </si>
+  <si>
+    <t>(a) the official bridge table from SIC to NAICS (b) Census Bureau Logitudinal Research Database plant level datafiles</t>
+  </si>
+  <si>
+    <t>How to create accurate time series data that converts frm SIC to NAICS classifications.</t>
+  </si>
+  <si>
+    <t>Using the 1997 bridge table from SIC to NAICS as a starting point, then recreate the table for previous yeats using LRD plant level data from across the U.S.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use plant level data from LRD to create a aggregate data set that can be used to correspond older SIC job codes to newer NAICS codes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demonstrates how to correspond codes from different classification systems as well as a method to assign wieghts when a new code may be made up of several older ones. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This paper showed how to create correspondence tables goiong backward, but also demonstrated that the further back in time one goes, the more challenging it becomes to create accurate correspndence. </t>
   </si>
 </sst>
 </file>
@@ -439,8 +511,8 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,8 +576,26 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -521,8 +611,26 @@
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -537,6 +645,24 @@
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -555,6 +681,12 @@
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -571,6 +703,24 @@
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>